<commit_message>
all api are connected to frontend and now all pages till creative thinking works
</commit_message>
<xml_diff>
--- a/preprocessing_scripts/instrument.xlsx
+++ b/preprocessing_scripts/instrument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varshahindupur/Downloads/RA_Online_Instrument/preprocessing_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E580BF4-5D81-5346-A01A-D103B7D0A37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA50887-8748-6B44-AF77-53F18C51F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,10 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,9 +478,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" customWidth="1"/>
+    <col min="7" max="7" width="4.5" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -535,7 +552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -557,7 +574,7 @@
       <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated excel sheet with new data
</commit_message>
<xml_diff>
--- a/preprocessing_scripts/instrument.xlsx
+++ b/preprocessing_scripts/instrument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varshahindupur/Downloads/RA_Online_Instrument/preprocessing_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA50887-8748-6B44-AF77-53F18C51F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C003550-96D8-6C46-BFD5-507DD347725F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>prolific_id</t>
   </si>
@@ -76,40 +76,127 @@
     <t>responses.question_10</t>
   </si>
   <si>
-    <t>123</t>
+    <t>responses.question_question1</t>
+  </si>
+  <si>
+    <t>responses.question_question2</t>
+  </si>
+  <si>
+    <t>responses.question_question3</t>
+  </si>
+  <si>
+    <t>responses.question_question4</t>
+  </si>
+  <si>
+    <t>responses.question_question5</t>
+  </si>
+  <si>
+    <t>responses.question_question6</t>
+  </si>
+  <si>
+    <t>responses.question_question7</t>
+  </si>
+  <si>
+    <t>responses.question_question8</t>
+  </si>
+  <si>
+    <t>responses.question_question9</t>
+  </si>
+  <si>
+    <t>responses.question_question10</t>
+  </si>
+  <si>
+    <t>responses.question_question11</t>
+  </si>
+  <si>
+    <t>r4r4r</t>
   </si>
   <si>
     <t>First-Consent</t>
   </si>
   <si>
-    <t>66b2e0fa0b5684fe460b641f</t>
-  </si>
-  <si>
-    <t>2024-08-07T02:50:34.315Z</t>
+    <t>66bab2026d6168e57c918a2e</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:08:18.367Z</t>
+  </si>
+  <si>
+    <t>Financial-Literacy</t>
+  </si>
+  <si>
+    <t>66bab20c6d6168e57c918a30</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:08:28.737Z</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>option3</t>
   </si>
   <si>
     <t>Paper-Folding-Test-1</t>
   </si>
   <si>
-    <t>66b2e1279c0009d39f467edb</t>
-  </si>
-  <si>
-    <t>2024-08-07T02:51:19.842Z</t>
+    <t>66bab2cebe2f8ac6f28f7798</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:11:42.015Z</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>Paper-Folding-Test-2</t>
   </si>
   <si>
-    <t>66b2e13a9c0009d39f467edd</t>
-  </si>
-  <si>
-    <t>2024-08-07T02:51:38.259Z</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>66bab317be2f8ac6f28f779a</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:12:55.876Z</t>
+  </si>
+  <si>
+    <t>Sample-Rotation-Test</t>
+  </si>
+  <si>
+    <t>66bab336be2f8ac6f28f779c</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:13:26.178Z</t>
+  </si>
+  <si>
+    <t>same,different,same,different,same,different,same,different</t>
+  </si>
+  <si>
+    <t>Rotation-Test-1</t>
+  </si>
+  <si>
+    <t>66bab3e6be2f8ac6f28f779e</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:16:22.333Z</t>
+  </si>
+  <si>
+    <t>Rotation-Test-2</t>
+  </si>
+  <si>
+    <t>66bab4a5be2f8ac6f28f77a0</t>
+  </si>
+  <si>
+    <t>2024-08-13T01:19:33.063Z</t>
+  </si>
+  <si>
+    <t>same,different,same,same,different,different,same,different</t>
   </si>
 </sst>
 </file>
@@ -128,7 +215,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,13 +252,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,27 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="3.83203125" customWidth="1"/>
-    <col min="7" max="7" width="4.5" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="19" max="19" width="50.33203125" customWidth="1"/>
+    <col min="20" max="20" width="61.1640625" customWidth="1"/>
+    <col min="21" max="21" width="48.6640625" customWidth="1"/>
+    <col min="22" max="22" width="51.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,13 +626,46 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -566,128 +674,310 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>2.8780000000000001</v>
+        <v>18.18</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>17.908999999999999</v>
+        <v>10.132</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>15.663</v>
+        <v>190.61099999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>19.344999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>30.04</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>168.36099999999999</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" t="s">
+        <v>51</v>
+      </c>
+      <c r="X7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>184.178</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" t="s">
+        <v>51</v>
+      </c>
+      <c r="U8" t="s">
+        <v>51</v>
+      </c>
+      <c r="V8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>